<commit_message>
lien sio chat et tab
</commit_message>
<xml_diff>
--- a/ressources/fiche exam/tab exam.xlsx
+++ b/ressources/fiche exam/tab exam.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swann\Desktop\code\portfolio\portfolio\ressources\fiche exam\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F26104-11C9-46C2-B10B-4DD6ACEAECA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Tableau de synthèse Épreuve E4'!$A$1:$H$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$16</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -25,60 +30,60 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
-    <t xml:space="preserve">BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
+    <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
   <si>
-    <t xml:space="preserve">SESSION 2022</t>
+    <t>SESSION 2022</t>
   </si>
   <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
   </si>
   <si>
-    <t xml:space="preserve">NOM et prénom : Baste Vergez</t>
+    <t>NOM et prénom : Baste Vergez</t>
   </si>
   <si>
-    <t xml:space="preserve">N° candidat : 02148340444</t>
+    <t>N° candidat : 02148340444</t>
   </si>
   <si>
-    <t xml:space="preserve">Centre de formation :</t>
+    <t>Centre de formation :</t>
   </si>
   <si>
-    <t xml:space="preserve">Option :</t>
+    <t>Option :</t>
   </si>
   <si>
-    <t xml:space="preserve">▢ SISR</t>
+    <t>▢ SISR</t>
   </si>
   <si>
-    <t xml:space="preserve">▢ SLAM</t>
+    <t>▢ SLAM</t>
   </si>
   <si>
-    <t xml:space="preserve">Compétences mises en œuvre
+    <t>Compétences mises en œuvre
 Réalisations professionnelles
 (intitulé et liste des documents et productions associés)</t>
   </si>
   <si>
-    <t xml:space="preserve">Période (sous la forme du JJ/MM/AA au JJ/MM/AA)</t>
+    <t>Période (sous la forme du JJ/MM/AA au JJ/MM/AA)</t>
   </si>
   <si>
-    <t xml:space="preserve">Gérer le patrimoine informatique</t>
+    <t>Gérer le patrimoine informatique</t>
   </si>
   <si>
-    <t xml:space="preserve">Répondre aux incidents et aux demandes d’assistance et d’évolution</t>
+    <t>Répondre aux incidents et aux demandes d’assistance et d’évolution</t>
   </si>
   <si>
-    <t xml:space="preserve">Développer la présence en ligne de l’organisation</t>
+    <t>Développer la présence en ligne de l’organisation</t>
   </si>
   <si>
-    <t xml:space="preserve">Travailler en mode projet</t>
+    <t>Travailler en mode projet</t>
   </si>
   <si>
-    <t xml:space="preserve">Mettre à disposition des utilisateurs un service informatique</t>
+    <t>Mettre à disposition des utilisateurs un service informatique</t>
   </si>
   <si>
-    <t xml:space="preserve">Organiser son développement professionnel</t>
+    <t>Organiser son développement professionnel</t>
   </si>
   <si>
-    <t xml:space="preserve">▸Recenser et identifier les ressources numériques 
+    <t>▸Recenser et identifier les ressources numériques 
 ▸Exploiter des référentiels, normes et standards adoptés par le prestataire informatique
 ▸Mettre en place et vérifier les niveaux d’habilitation associés à un service
 ▸Vérifier les conditions de la continuité d’un service informatique
@@ -86,27 +91,27 @@
 ▸Vérifier le respect des règles d’utilisation des ressources numériques</t>
   </si>
   <si>
-    <t xml:space="preserve">▸Collecter, suivre et orienter des demandes 
+    <t>▸Collecter, suivre et orienter des demandes 
 ▸Traiter des demandes concernant les services réseau et système, applicatifs
 ▸Traiter des demandes concernant les applications</t>
   </si>
   <si>
-    <t xml:space="preserve">▸Participer à la valorisation de l’image de l’organisation sur les médias numériques en tenant compte du cadre juridique et des enjeux économiques
+    <t>▸Participer à la valorisation de l’image de l’organisation sur les médias numériques en tenant compte du cadre juridique et des enjeux économiques
 ▸Référencer les services en ligne de l’organisation et mesurer leur visibilité.
 ▸Participer à l’évolution d’un site Web exploitant les données de l’organisation.</t>
   </si>
   <si>
-    <t xml:space="preserve">▸Analyser les objectifs et les modalités d’organisation d’un projet
+    <t>▸Analyser les objectifs et les modalités d’organisation d’un projet
 ▸Planifier les activités
 ▸Évaluer les indicateurs de suivi d’un projet et analyser les écarts</t>
   </si>
   <si>
-    <t xml:space="preserve">▸Réaliser les tests d’intégration et d’acceptation d’un service
+    <t>▸Réaliser les tests d’intégration et d’acceptation d’un service
 ▸Déployer un service
 ▸Accompagner les utilisateurs dans la mise en place d’un service</t>
   </si>
   <si>
-    <t xml:space="preserve">▸Mettre en place son environnement d’apprentissage personnel
+    <t>▸Mettre en place son environnement d’apprentissage personnel
 ▸Mettre en œuvre des outils et stratégies de veille informationnelle
 ▸Gérer son identité professionnelle
 ▸Développer son projet professionnel</t>
@@ -116,192 +121,128 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">SIO Chat (Site de messagerie en ligne)</t>
+    <t>SIO Chat (Site de messagerie en ligne)</t>
   </si>
   <si>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="11"/>
         <rFont val="Arial"/>
-        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">GLPI (Gestion du </t>
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="11"/>
         <rFont val="Arial"/>
-        <family val="0"/>
       </rPr>
-      <t xml:space="preserve">Patrimoine Informatique)</t>
+      <t>Patrimoine Informatique)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Ma veille technologique</t>
+    <t>Ma veille technologique</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mon portfolio</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> et mes réseaux</t>
-    </r>
+    <t>Réalisations en milieu professionnel en cours de première année</t>
   </si>
   <si>
-    <t xml:space="preserve">Réalisations en milieu professionnel en cours de première année</t>
+    <t>Réalisations en milieu professionnel en cours de seconde année</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Stoolz</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> (site de seconde main)</t>
-    </r>
+    <t>Projet alternance (Gestion de procédure en No Code)</t>
   </si>
   <si>
-    <t xml:space="preserve">Réalisations en milieu professionnel en cours de seconde année</t>
+    <t>Mon portfolio et mes réseaux</t>
   </si>
   <si>
-    <t xml:space="preserve">Projet alternance (Gestion de procédure en No Code)</t>
+    <t>Stoolz (site de seconde main)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* \-??\ [$€-1]_-"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* \-??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="20"/>
-      <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="18"/>
+      <b/>
+      <sz val="14"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="16"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -314,14 +255,14 @@
     </fill>
   </fills>
   <borders count="15">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -336,7 +277,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -349,7 +290,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -360,7 +301,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FF4A452A"/>
@@ -373,7 +314,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="true">
+    <border diagonalDown="1">
       <left style="medium">
         <color rgb="FF4A452A"/>
       </left>
@@ -388,7 +329,7 @@
         <color rgb="FF4A452A"/>
       </diagonal>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -403,7 +344,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -418,7 +359,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -433,7 +374,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -446,7 +387,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -459,7 +400,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF4A452A"/>
       </left>
@@ -474,7 +415,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF4A452A"/>
       </left>
@@ -489,7 +430,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -504,7 +445,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF4A452A"/>
       </left>
@@ -520,149 +461,96 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="3">
+    <cellStyle name="Euro" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Euro" xfId="20"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -721,14 +609,30 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF4A452A"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="twoCell">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>43200</xdr:colOff>
@@ -741,9 +645,15 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>458280</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvPr id="2" name="Forme libre : forme 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -760,9 +670,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 398160 h 397800"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="0" y="0"/>
               </a:moveTo>
@@ -833,28 +744,34 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>251280</xdr:colOff>
+      <xdr:colOff>48080</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1134000</xdr:colOff>
+      <xdr:colOff>1206500</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>415440</xdr:rowOff>
+      <xdr:rowOff>440840</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvPr id="3" name="Forme libre : forme 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11255760" y="7680960"/>
-          <a:ext cx="882720" cy="276840"/>
+          <a:off x="10449380" y="7594600"/>
+          <a:ext cx="1158420" cy="390040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -865,9 +782,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 277200 h 276840"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="43200" y="0"/>
               </a:moveTo>
@@ -921,10 +839,17 @@
         </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>25920</xdr:colOff>
@@ -937,9 +862,15 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>458640</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvPr id="4" name="Forme libre : forme 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -956,9 +887,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 415800 h 415440"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="0" y="0"/>
               </a:moveTo>
@@ -1024,7 +956,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>34560</xdr:colOff>
@@ -1037,9 +969,15 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>441000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvPr id="5" name="Forme libre : forme 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1056,9 +994,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 389520 h 389160"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="43200" y="0"/>
               </a:moveTo>
@@ -1134,7 +1073,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>147240</xdr:colOff>
@@ -1147,9 +1086,15 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>424080</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvPr id="6" name="Forme libre : forme 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1166,9 +1111,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 268560 h 268200"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="0" y="0"/>
               </a:moveTo>
@@ -1218,7 +1164,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>173160</xdr:colOff>
@@ -1231,9 +1177,15 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>371880</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvPr id="7" name="Forme libre : forme 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1250,9 +1202,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 216360 h 216000"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="43200" y="0"/>
               </a:moveTo>
@@ -1298,7 +1251,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>25920</xdr:colOff>
@@ -1311,9 +1264,15 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>458640</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name=""/>
+        <xdr:cNvPr id="8" name="Forme libre : forme 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1330,9 +1289,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 433080 h 432720"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="0" y="0"/>
               </a:moveTo>
@@ -1403,7 +1363,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>95400</xdr:colOff>
@@ -1416,9 +1376,15 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>441000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name=""/>
+        <xdr:cNvPr id="9" name="Forme libre : forme 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1435,9 +1401,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 398160 h 397800"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="43200" y="0"/>
               </a:moveTo>
@@ -1508,7 +1475,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>34560</xdr:colOff>
@@ -1521,9 +1488,15 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>415080</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name=""/>
+        <xdr:cNvPr id="10" name="Forme libre : forme 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1540,9 +1513,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 372240 h 371880"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="0" y="0"/>
               </a:moveTo>
@@ -1603,7 +1577,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1186200</xdr:colOff>
@@ -1616,9 +1590,15 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>475920</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name=""/>
+        <xdr:cNvPr id="11" name="Forme libre : forme 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1635,9 +1615,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 424440 h 424080"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="43200" y="0"/>
               </a:moveTo>
@@ -1699,7 +1680,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>43200</xdr:colOff>
@@ -1712,9 +1693,15 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>389160</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name=""/>
+        <xdr:cNvPr id="12" name="Forme libre : forme 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1731,9 +1718,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 346320 h 345960"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="0" y="0"/>
               </a:moveTo>
@@ -1804,7 +1792,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>69120</xdr:colOff>
@@ -1817,9 +1805,15 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>441000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name=""/>
+        <xdr:cNvPr id="13" name="Forme libre : forme 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1836,9 +1830,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 406800 h 406440"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="43200" y="0"/>
               </a:moveTo>
@@ -1910,7 +1905,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1238400</xdr:colOff>
@@ -1923,9 +1918,15 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>389160</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name=""/>
+        <xdr:cNvPr id="14" name="Forme libre : forme 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1942,9 +1943,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 363600 h 363240"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="0" y="0"/>
               </a:moveTo>
@@ -2010,7 +2012,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>86760</xdr:colOff>
@@ -2023,9 +2025,15 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>415080</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name=""/>
+        <xdr:cNvPr id="15" name="Forme libre : forme 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2042,9 +2050,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 363600 h 363240"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="43200" y="0"/>
               </a:moveTo>
@@ -2110,7 +2119,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>17280</xdr:colOff>
@@ -2123,9 +2132,15 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>397800</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name=""/>
+        <xdr:cNvPr id="16" name="Forme libre : forme 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2142,9 +2157,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 380880 h 380520"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="0" y="0"/>
               </a:moveTo>
@@ -2214,7 +2230,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>86760</xdr:colOff>
@@ -2227,9 +2243,15 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>467280</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name=""/>
+        <xdr:cNvPr id="17" name="Forme libre : forme 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2246,9 +2268,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 424440 h 424080"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="43200" y="0"/>
               </a:moveTo>
@@ -2323,7 +2346,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>8640</xdr:colOff>
@@ -2336,9 +2359,15 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>467280</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name=""/>
+        <xdr:cNvPr id="18" name="Forme libre : forme 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2355,9 +2384,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 433080 h 432720"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="0" y="864"/>
               </a:moveTo>
@@ -2424,7 +2454,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>43200</xdr:colOff>
@@ -2437,9 +2467,15 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>432360</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name=""/>
+        <xdr:cNvPr id="19" name="Forme libre : forme 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2456,9 +2492,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 380880 h 380520"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="43200" y="0"/>
               </a:moveTo>
@@ -2529,7 +2566,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>34560</xdr:colOff>
@@ -2542,9 +2579,15 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>432720</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name=""/>
+        <xdr:cNvPr id="20" name="Forme libre : forme 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2561,9 +2604,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 424440 h 424080"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="0" y="0"/>
               </a:moveTo>
@@ -2614,7 +2658,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>25920</xdr:colOff>
@@ -2627,9 +2671,15 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>328680</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name=""/>
+        <xdr:cNvPr id="21" name="Forme libre : forme 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2646,9 +2696,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 277200 h 276840"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="43200" y="0"/>
               </a:moveTo>
@@ -2716,9 +2767,15 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>428760</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name=""/>
+        <xdr:cNvPr id="22" name="Forme libre : forme 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2735,9 +2792,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 424440 h 424080"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="43200" y="0"/>
               </a:moveTo>
@@ -2820,14 +2878,20 @@
       <xdr:rowOff>12960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1305720</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3970</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>507240</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name=""/>
+        <xdr:cNvPr id="23" name="Forme libre : forme 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2844,9 +2908,10 @@
             <a:gd name="textAreaBottom" fmla="*/ 494280 h 494280"/>
           </a:gdLst>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
-            <a:path fill="none" w="43200" h="43200">
+            <a:path w="43200" h="43200" fill="none">
               <a:moveTo>
                 <a:pt x="43200" y="0"/>
               </a:moveTo>
@@ -2921,327 +2986,837 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1241880</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1155700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>453540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Forme libre : forme 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642EC700-62A9-4ECB-AAE0-C09E9CEA45A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6664780" y="7607300"/>
+          <a:ext cx="1158420" cy="390040"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="textAreaLeft" fmla="*/ 0 w 882720"/>
+            <a:gd name="textAreaRight" fmla="*/ 883080 w 882720"/>
+            <a:gd name="textAreaTop" fmla="*/ 0 h 276840"/>
+            <a:gd name="textAreaBottom" fmla="*/ 277200 h 276840"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
+          <a:pathLst>
+            <a:path w="43200" h="43200" fill="none">
+              <a:moveTo>
+                <a:pt x="43200" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="41082" y="0"/>
+                <a:pt x="37270" y="4049"/>
+                <a:pt x="35152" y="8099"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="32188" y="12149"/>
+                <a:pt x="28800" y="16199"/>
+                <a:pt x="25835" y="20249"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="23294" y="22950"/>
+                <a:pt x="19905" y="25649"/>
+                <a:pt x="17788" y="28350"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="13976" y="31050"/>
+                <a:pt x="11858" y="33749"/>
+                <a:pt x="8470" y="36450"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="4658" y="40500"/>
+                <a:pt x="2117" y="41850"/>
+                <a:pt x="0" y="43200"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>176480</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>84440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1163240</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>482240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Forme libre : forme 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E67D7FC8-4557-4F13-9E19-BEE9E8C66520}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6843980" y="7628240"/>
+          <a:ext cx="986760" cy="397800"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="textAreaLeft" fmla="*/ 0 w 986760"/>
+            <a:gd name="textAreaRight" fmla="*/ 987120 w 986760"/>
+            <a:gd name="textAreaTop" fmla="*/ 0 h 397800"/>
+            <a:gd name="textAreaBottom" fmla="*/ 398160 h 397800"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
+          <a:pathLst>
+            <a:path w="43200" h="43200" fill="none">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="3031" y="1878"/>
+                <a:pt x="5684" y="4695"/>
+                <a:pt x="7200" y="6573"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="9473" y="8452"/>
+                <a:pt x="10989" y="10330"/>
+                <a:pt x="12884" y="12208"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="14400" y="14086"/>
+                <a:pt x="15915" y="16904"/>
+                <a:pt x="17431" y="18782"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="19326" y="20660"/>
+                <a:pt x="20842" y="22539"/>
+                <a:pt x="22736" y="24417"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="24252" y="26295"/>
+                <a:pt x="26147" y="27234"/>
+                <a:pt x="28042" y="29113"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="29936" y="30052"/>
+                <a:pt x="32210" y="31930"/>
+                <a:pt x="34105" y="32869"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="35621" y="34747"/>
+                <a:pt x="37136" y="36626"/>
+                <a:pt x="38652" y="38504"/>
+              </a:cubicBezTo>
+              <a:quadBezTo>
+                <a:pt x="40547" y="41321"/>
+                <a:pt x="43200" y="43200"/>
+              </a:quadBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:AQ62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="70.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="9" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="44" style="1" width="10.85"/>
+    <col min="1" max="1" width="70.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="7"/>
+    <col min="3" max="8" width="18.7109375" style="7" customWidth="1"/>
+    <col min="9" max="43" width="11.42578125" customWidth="1"/>
+    <col min="44" max="16384" width="10.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="41.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:13" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
-    <row r="3" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" s="13" customFormat="true" ht="324.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="11" t="s">
+    <row r="6" spans="1:13" s="15" customFormat="1" ht="324.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="14" t="s">
         <v>22</v>
       </c>
+      <c r="L6" s="24"/>
     </row>
-    <row r="7" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:13" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
-    <row r="8" s="13" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:13" s="15" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
     </row>
-    <row r="9" s="13" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:13" s="15" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
     </row>
-    <row r="10" s="13" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:13" s="15" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
     </row>
-    <row r="11" s="13" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:13" s="15" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+    </row>
+    <row r="12" spans="1:13" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="19"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
-    <row r="12" s="13" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21" t="s">
+    <row r="13" spans="1:13" s="15" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:13" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
-    <row r="13" s="13" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="s">
+    <row r="15" spans="1:13" s="15" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="19"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="20"/>
     </row>
-    <row r="14" s="13" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
+    <row r="16" spans="1:13" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
     </row>
-    <row r="15" s="13" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="19"/>
-    </row>
-    <row r="16" s="13" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-    </row>
-    <row r="17" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="55" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A12:H12"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A14:H14"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A11" r:id="rId1" display="Mon portfolio"/>
-    <hyperlink ref="A13" r:id="rId2" display="Stoolz"/>
+    <hyperlink ref="A11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A13" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A8" r:id="rId3" display="SIO Chat" xr:uid="{A6631B1B-DCFF-4C91-82A5-B5E32BCFC47E}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.196527777777778" right="0.196527777777778" top="0.196527777777778" bottom="0.196527777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>